<commit_message>
backup; metadata now for R8043 and R8521
</commit_message>
<xml_diff>
--- a/exp_design/NGS_Samples_Philipp_mRNAseq_all.xlsx
+++ b/exp_design/NGS_Samples_Philipp_mRNAseq_all.xlsx
@@ -8,23 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/groups/cochella/jiwang/Projects/Philipp/smallRNA_analysis_philipp/exp_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEE780C7-93D2-5F47-9550-A8BD995801DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8ED9561-65B3-B644-B4B7-B4EBB616B1F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43560" yWindow="-5580" windowWidth="30340" windowHeight="17440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39820" yWindow="-12520" windowWidth="37420" windowHeight="29860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="227">
   <si>
     <t>Sample ID</t>
   </si>
@@ -502,13 +496,226 @@
   </si>
   <si>
     <t>Samples E &amp; F are 20% of the corresponding sRNAseq sample (original # of embryos divided by 5)</t>
+  </si>
+  <si>
+    <t>Conc. FA [ng/ul]</t>
+  </si>
+  <si>
+    <t>Add for 30 ul</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>5001 / 7049</t>
+  </si>
+  <si>
+    <t>8521 / M9011</t>
+  </si>
+  <si>
+    <t>HCYCVBGXC</t>
+  </si>
+  <si>
+    <t>20 degree</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>5002 / 7050</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>5003 / 7051</t>
+  </si>
+  <si>
+    <t>MT14533</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>5004 / 7052</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>5001 / 7053</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>5002 / 7054</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>5003 / 7055</t>
+  </si>
+  <si>
+    <t>25 degree</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>5004 / 7056</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>5001 / 7057</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>5002 / 7058</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>5003 / 7059</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>5004 / 7060</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>5001 / 7061</t>
+  </si>
+  <si>
+    <t>Failed library prep</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>5003 / 7063</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>5004 / 7064</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>5001 / 7065</t>
+  </si>
+  <si>
+    <t>failed library prep</t>
+  </si>
+  <si>
+    <t>5002 / 7066</t>
+  </si>
+  <si>
+    <t>190 cell</t>
+  </si>
+  <si>
+    <t>5003 / 7067</t>
+  </si>
+  <si>
+    <t>5004 / 7068</t>
+  </si>
+  <si>
+    <t>Bean</t>
+  </si>
+  <si>
+    <t>5001 / 7069</t>
+  </si>
+  <si>
+    <t>5002 / 7070</t>
+  </si>
+  <si>
+    <t>2-fold</t>
+  </si>
+  <si>
+    <t>5003 / 7071</t>
+  </si>
+  <si>
+    <t>5004 / 7072</t>
+  </si>
+  <si>
+    <t>MLC1800</t>
+  </si>
+  <si>
+    <t>5001 / 7073</t>
+  </si>
+  <si>
+    <t>5002 / 7074</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>5003 / 7075</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>5004 / 7076</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>5001 / 7077</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t xml:space="preserve">per sample </t>
+  </si>
+  <si>
+    <t>mir-35 fam mutant (mom without balancer)</t>
+  </si>
+  <si>
+    <t>total Volume final</t>
+  </si>
+  <si>
+    <t>30 uL</t>
+  </si>
+  <si>
+    <t>Water inout into library prep</t>
+  </si>
+  <si>
+    <t>everything at 20</t>
+  </si>
+  <si>
+    <t>Moms shifted to 25 as L4s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -537,6 +744,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -558,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -594,6 +808,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,20 +1091,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:V105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" style="2" customWidth="1"/>
     <col min="2" max="3" width="23.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" style="2" customWidth="1"/>
     <col min="5" max="6" width="19.1640625" style="2" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="16.5" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
@@ -898,7 +1115,7 @@
     <col min="19" max="24" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -959,8 +1176,14 @@
       <c r="T1" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>156</v>
+      </c>
+      <c r="V1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>44</v>
       </c>
@@ -1020,7 +1243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
@@ -1079,7 +1302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1138,7 +1361,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -1197,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1256,7 +1479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>44</v>
       </c>
@@ -1315,7 +1538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1374,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
@@ -1433,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1492,7 +1715,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1552,7 +1775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1612,7 +1835,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -1672,7 +1895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>44</v>
       </c>
@@ -1732,7 +1955,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +2014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -1850,7 +2073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1909,7 +2132,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -1968,7 +2191,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -2027,7 +2250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -2086,7 +2309,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
@@ -2146,7 +2369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>44</v>
       </c>
@@ -2206,7 +2429,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -2266,7 +2489,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -2326,7 +2549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
@@ -2385,7 +2608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -2445,7 +2668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
@@ -2504,7 +2727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -2563,7 +2786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
@@ -2622,7 +2845,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -2681,7 +2904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -2740,7 +2963,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
@@ -2799,7 +3022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>44</v>
       </c>
@@ -2858,7 +3081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
@@ -2917,7 +3140,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -2977,7 +3200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -3037,7 +3260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -3097,7 +3320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -3157,7 +3380,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -3216,7 +3439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -3275,7 +3498,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -3334,7 +3557,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -3393,7 +3616,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -3452,7 +3675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -3511,7 +3734,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
@@ -3570,7 +3793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -3629,7 +3852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>44</v>
       </c>
@@ -3688,7 +3911,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
@@ -3747,7 +3970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>44</v>
       </c>
@@ -3806,615 +4029,1963 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:20">
-      <c r="H50" s="5"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-    </row>
-    <row r="51" spans="1:20">
-      <c r="H51" s="5"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-    </row>
-    <row r="52" spans="1:20">
-      <c r="A52" s="10" t="s">
+    <row r="50" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H50" s="3">
+        <v>99987</v>
+      </c>
+      <c r="I50" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" t="s">
+        <v>14</v>
+      </c>
+      <c r="K50" t="s">
+        <v>48</v>
+      </c>
+      <c r="L50" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M50" t="s">
+        <v>18</v>
+      </c>
+      <c r="N50" s="2"/>
+      <c r="O50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R50" s="3">
+        <v>0</v>
+      </c>
+      <c r="S50" s="7">
+        <v>24</v>
+      </c>
+      <c r="T50" s="3">
+        <v>20</v>
+      </c>
+      <c r="U50" s="5">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="V50" s="14">
+        <f>$V$33/U50*30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H51" s="3">
+        <v>99988</v>
+      </c>
+      <c r="I51" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" t="s">
+        <v>14</v>
+      </c>
+      <c r="K51" t="s">
+        <v>48</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M51" t="s">
+        <v>18</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R51" s="3">
+        <v>4</v>
+      </c>
+      <c r="S51" s="9">
+        <v>15</v>
+      </c>
+      <c r="T51" s="3">
+        <v>21</v>
+      </c>
+      <c r="U51" s="5">
+        <v>1.81</v>
+      </c>
+      <c r="V51" s="14">
+        <f t="shared" ref="V51:V77" si="0">$V$33/U51*30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H52" s="3">
+        <v>99989</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" t="s">
+        <v>14</v>
+      </c>
+      <c r="K52" t="s">
+        <v>48</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M52" t="s">
+        <v>18</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R52" s="3">
+        <v>0</v>
+      </c>
+      <c r="S52" s="9">
+        <v>18</v>
+      </c>
+      <c r="T52" s="3">
+        <v>20</v>
+      </c>
+      <c r="U52" s="5">
+        <v>2.08</v>
+      </c>
+      <c r="V52" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H53" s="3">
+        <v>99990</v>
+      </c>
+      <c r="I53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" t="s">
+        <v>14</v>
+      </c>
+      <c r="K53" t="s">
+        <v>48</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M53" t="s">
+        <v>18</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R53" s="3">
+        <v>4</v>
+      </c>
+      <c r="S53" s="9">
+        <v>24</v>
+      </c>
+      <c r="T53" s="3">
+        <v>21</v>
+      </c>
+      <c r="U53" s="2">
+        <v>2.09</v>
+      </c>
+      <c r="V53" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H54" s="3">
+        <v>99991</v>
+      </c>
+      <c r="I54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" t="s">
+        <v>48</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M54" t="s">
+        <v>18</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R54" s="3">
+        <v>0</v>
+      </c>
+      <c r="S54" s="9">
+        <v>20</v>
+      </c>
+      <c r="T54" s="3">
+        <v>20</v>
+      </c>
+      <c r="U54" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="V54" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H55" s="3">
+        <v>99992</v>
+      </c>
+      <c r="I55" t="s">
+        <v>13</v>
+      </c>
+      <c r="J55" t="s">
+        <v>14</v>
+      </c>
+      <c r="K55" t="s">
+        <v>48</v>
+      </c>
+      <c r="L55" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M55" t="s">
+        <v>18</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q55" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R55" s="3">
+        <v>4</v>
+      </c>
+      <c r="S55" s="9">
+        <v>25</v>
+      </c>
+      <c r="T55" s="3">
+        <v>21</v>
+      </c>
+      <c r="U55" s="2">
+        <v>1.83</v>
+      </c>
+      <c r="V55" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H56" s="3">
+        <v>99993</v>
+      </c>
+      <c r="I56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" t="s">
+        <v>14</v>
+      </c>
+      <c r="K56" t="s">
+        <v>48</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M56" t="s">
+        <v>18</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R56" s="3">
+        <v>0</v>
+      </c>
+      <c r="S56" s="9">
+        <v>30</v>
+      </c>
+      <c r="T56" s="3">
+        <v>19</v>
+      </c>
+      <c r="U56" s="2">
+        <v>2.14</v>
+      </c>
+      <c r="V56" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H57" s="3">
+        <v>99994</v>
+      </c>
+      <c r="I57" t="s">
+        <v>13</v>
+      </c>
+      <c r="J57" t="s">
+        <v>14</v>
+      </c>
+      <c r="K57" t="s">
+        <v>48</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M57" t="s">
+        <v>18</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R57" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="S57" s="9">
+        <v>18</v>
+      </c>
+      <c r="T57" s="3">
+        <v>21</v>
+      </c>
+      <c r="U57" s="2">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="V57" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H58" s="3">
+        <v>99995</v>
+      </c>
+      <c r="I58" t="s">
+        <v>13</v>
+      </c>
+      <c r="J58" t="s">
+        <v>14</v>
+      </c>
+      <c r="K58" t="s">
+        <v>48</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M58" t="s">
+        <v>18</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R58" s="3">
+        <v>0</v>
+      </c>
+      <c r="S58" s="7">
+        <v>40</v>
+      </c>
+      <c r="T58" s="3">
+        <v>19</v>
+      </c>
+      <c r="U58" s="2">
+        <v>1.42</v>
+      </c>
+      <c r="V58" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H59" s="3">
+        <v>99996</v>
+      </c>
+      <c r="I59" t="s">
+        <v>13</v>
+      </c>
+      <c r="J59" t="s">
+        <v>14</v>
+      </c>
+      <c r="K59" t="s">
+        <v>48</v>
+      </c>
+      <c r="L59" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M59" t="s">
+        <v>18</v>
+      </c>
+      <c r="N59" s="4"/>
+      <c r="O59" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R59" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="S59" s="7">
+        <v>23</v>
+      </c>
+      <c r="T59" s="3">
+        <v>21</v>
+      </c>
+      <c r="U59" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="V59" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H60" s="3">
+        <v>99997</v>
+      </c>
+      <c r="I60" t="s">
+        <v>13</v>
+      </c>
+      <c r="J60" t="s">
+        <v>14</v>
+      </c>
+      <c r="K60" t="s">
+        <v>48</v>
+      </c>
+      <c r="L60" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M60" t="s">
+        <v>18</v>
+      </c>
+      <c r="N60" s="4"/>
+      <c r="O60" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R60" s="3">
+        <v>0</v>
+      </c>
+      <c r="S60" s="7">
+        <v>40</v>
+      </c>
+      <c r="T60" s="3">
+        <v>20</v>
+      </c>
+      <c r="U60" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="V60" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H61" s="3">
+        <v>99998</v>
+      </c>
+      <c r="I61" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61" t="s">
+        <v>14</v>
+      </c>
+      <c r="K61" t="s">
+        <v>48</v>
+      </c>
+      <c r="L61" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M61" t="s">
+        <v>18</v>
+      </c>
+      <c r="N61" s="4"/>
+      <c r="O61" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q61" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R61" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="S61" s="7">
+        <v>27</v>
+      </c>
+      <c r="T61" s="3">
+        <v>21</v>
+      </c>
+      <c r="U61" s="2">
+        <v>2.04</v>
+      </c>
+      <c r="V61" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H62" s="3">
+        <v>99999</v>
+      </c>
+      <c r="I62" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" t="s">
+        <v>14</v>
+      </c>
+      <c r="K62" t="s">
+        <v>48</v>
+      </c>
+      <c r="L62" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M62" t="s">
+        <v>18</v>
+      </c>
+      <c r="N62" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O62" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P62" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q62" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="R62" s="3">
+        <v>0</v>
+      </c>
+      <c r="S62" s="7">
+        <v>36</v>
+      </c>
+      <c r="T62" s="3">
+        <v>21</v>
+      </c>
+      <c r="U62" s="5">
+        <v>2.33</v>
+      </c>
+      <c r="V62" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H63" s="3">
+        <v>100000</v>
+      </c>
+      <c r="I63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" t="s">
+        <v>14</v>
+      </c>
+      <c r="K63" t="s">
+        <v>48</v>
+      </c>
+      <c r="L63" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M63" t="s">
+        <v>18</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T63" s="3">
+        <v>21</v>
+      </c>
+      <c r="U63" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="V63" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H64" s="3">
+        <v>100001</v>
+      </c>
+      <c r="I64" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" t="s">
+        <v>14</v>
+      </c>
+      <c r="K64" t="s">
+        <v>48</v>
+      </c>
+      <c r="L64" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M64" t="s">
+        <v>18</v>
+      </c>
+      <c r="O64" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S64" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T64" s="3">
+        <v>18</v>
+      </c>
+      <c r="U64" s="2">
+        <v>3.14</v>
+      </c>
+      <c r="V64" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H65" s="3">
+        <v>100002</v>
+      </c>
+      <c r="I65" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" t="s">
+        <v>14</v>
+      </c>
+      <c r="K65" t="s">
+        <v>48</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M65" t="s">
+        <v>18</v>
+      </c>
+      <c r="N65" t="s">
+        <v>198</v>
+      </c>
+      <c r="O65" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q65" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="R65" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="S65" s="9">
+        <v>32</v>
+      </c>
+      <c r="T65" s="3">
+        <v>21</v>
+      </c>
+      <c r="U65" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="V65" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H66" s="3">
+        <v>100003</v>
+      </c>
+      <c r="I66" t="s">
+        <v>13</v>
+      </c>
+      <c r="J66" t="s">
+        <v>14</v>
+      </c>
+      <c r="K66" t="s">
+        <v>48</v>
+      </c>
+      <c r="L66" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M66" t="s">
+        <v>18</v>
+      </c>
+      <c r="O66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P66" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R66" s="3">
+        <v>3</v>
+      </c>
+      <c r="S66" s="7">
+        <v>50</v>
+      </c>
+      <c r="T66" s="3">
+        <v>21</v>
+      </c>
+      <c r="U66" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="V66" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H67" s="3">
+        <v>100004</v>
+      </c>
+      <c r="I67" t="s">
+        <v>13</v>
+      </c>
+      <c r="J67" t="s">
+        <v>14</v>
+      </c>
+      <c r="K67" t="s">
+        <v>48</v>
+      </c>
+      <c r="L67" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M67" t="s">
+        <v>18</v>
+      </c>
+      <c r="O67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P67" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q67" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R67" s="3">
+        <v>3</v>
+      </c>
+      <c r="S67" s="7">
+        <v>50</v>
+      </c>
+      <c r="T67" s="3">
+        <v>19</v>
+      </c>
+      <c r="U67" s="2">
+        <v>0.84</v>
+      </c>
+      <c r="V67" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H68" s="3">
+        <v>100005</v>
+      </c>
+      <c r="I68" t="s">
+        <v>13</v>
+      </c>
+      <c r="J68" t="s">
+        <v>14</v>
+      </c>
+      <c r="K68" t="s">
+        <v>48</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M68" t="s">
+        <v>18</v>
+      </c>
+      <c r="N68" s="4"/>
+      <c r="O68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P68" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R68" s="3">
+        <v>5</v>
+      </c>
+      <c r="S68" s="7">
+        <v>50</v>
+      </c>
+      <c r="T68" s="3">
+        <v>21</v>
+      </c>
+      <c r="U68" s="2">
+        <v>1.76</v>
+      </c>
+      <c r="V68" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H69" s="3">
+        <v>100006</v>
+      </c>
+      <c r="I69" t="s">
+        <v>13</v>
+      </c>
+      <c r="J69" t="s">
+        <v>14</v>
+      </c>
+      <c r="K69" t="s">
+        <v>48</v>
+      </c>
+      <c r="L69" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M69" t="s">
+        <v>18</v>
+      </c>
+      <c r="N69" s="4"/>
+      <c r="O69" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P69" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q69" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R69" s="3">
+        <v>5</v>
+      </c>
+      <c r="S69" s="7">
+        <v>50</v>
+      </c>
+      <c r="T69" s="3">
+        <v>20</v>
+      </c>
+      <c r="U69" s="2">
+        <v>1.51</v>
+      </c>
+      <c r="V69" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H70" s="3">
+        <v>100007</v>
+      </c>
+      <c r="I70" t="s">
+        <v>13</v>
+      </c>
+      <c r="J70" t="s">
+        <v>14</v>
+      </c>
+      <c r="K70" t="s">
+        <v>48</v>
+      </c>
+      <c r="L70" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M70" t="s">
+        <v>18</v>
+      </c>
+      <c r="N70" s="4"/>
+      <c r="O70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P70" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q70" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R70" s="3">
+        <v>7</v>
+      </c>
+      <c r="S70" s="7">
+        <v>50</v>
+      </c>
+      <c r="T70" s="3">
+        <v>20</v>
+      </c>
+      <c r="U70" s="2">
+        <v>1.81</v>
+      </c>
+      <c r="V70" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H71" s="3">
+        <v>100008</v>
+      </c>
+      <c r="I71" t="s">
+        <v>13</v>
+      </c>
+      <c r="J71" t="s">
+        <v>14</v>
+      </c>
+      <c r="K71" t="s">
+        <v>48</v>
+      </c>
+      <c r="L71" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M71" t="s">
+        <v>18</v>
+      </c>
+      <c r="N71" s="4"/>
+      <c r="O71" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P71" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q71" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R71" s="3">
+        <v>7</v>
+      </c>
+      <c r="S71" s="7">
+        <v>50</v>
+      </c>
+      <c r="T71" s="3">
+        <v>18</v>
+      </c>
+      <c r="U71" s="2">
+        <v>1.98</v>
+      </c>
+      <c r="V71" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H72" s="3">
+        <v>100009</v>
+      </c>
+      <c r="I72" t="s">
+        <v>13</v>
+      </c>
+      <c r="J72" t="s">
+        <v>14</v>
+      </c>
+      <c r="K72" t="s">
+        <v>48</v>
+      </c>
+      <c r="L72" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M72" t="s">
+        <v>18</v>
+      </c>
+      <c r="O72" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P72" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q72" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R72" s="3">
+        <v>3</v>
+      </c>
+      <c r="S72" s="7">
+        <v>35</v>
+      </c>
+      <c r="T72" s="3">
+        <v>21</v>
+      </c>
+      <c r="U72" s="2">
+        <v>2.64</v>
+      </c>
+      <c r="V72" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H73" s="3">
+        <v>100010</v>
+      </c>
+      <c r="I73" t="s">
+        <v>13</v>
+      </c>
+      <c r="J73" t="s">
+        <v>14</v>
+      </c>
+      <c r="K73" t="s">
+        <v>48</v>
+      </c>
+      <c r="L73" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M73" t="s">
+        <v>18</v>
+      </c>
+      <c r="N73" s="2"/>
+      <c r="O73" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P73" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q73" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R73" s="3">
+        <v>3</v>
+      </c>
+      <c r="S73" s="9">
+        <v>35</v>
+      </c>
+      <c r="T73" s="3">
+        <v>21</v>
+      </c>
+      <c r="U73" s="2">
+        <v>1.78</v>
+      </c>
+      <c r="V73" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H74" s="3">
+        <v>100011</v>
+      </c>
+      <c r="I74" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" t="s">
+        <v>14</v>
+      </c>
+      <c r="K74" t="s">
+        <v>48</v>
+      </c>
+      <c r="L74" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M74" t="s">
+        <v>18</v>
+      </c>
+      <c r="O74" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P74" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q74" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R74" s="3">
+        <v>5</v>
+      </c>
+      <c r="S74" s="7">
+        <v>60</v>
+      </c>
+      <c r="T74" s="3">
+        <v>21</v>
+      </c>
+      <c r="U74" s="2">
+        <v>2.69</v>
+      </c>
+      <c r="V74" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H75" s="3">
+        <v>100012</v>
+      </c>
+      <c r="I75" t="s">
+        <v>13</v>
+      </c>
+      <c r="J75" t="s">
+        <v>14</v>
+      </c>
+      <c r="K75" t="s">
+        <v>48</v>
+      </c>
+      <c r="L75" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M75" t="s">
+        <v>18</v>
+      </c>
+      <c r="O75" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P75" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q75" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R75" s="3">
+        <v>5</v>
+      </c>
+      <c r="S75" s="7">
+        <v>60</v>
+      </c>
+      <c r="T75" s="3">
+        <v>21</v>
+      </c>
+      <c r="U75" s="2">
+        <v>2.56</v>
+      </c>
+      <c r="V75" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H76" s="3">
+        <v>100013</v>
+      </c>
+      <c r="I76" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" t="s">
+        <v>14</v>
+      </c>
+      <c r="K76" t="s">
+        <v>48</v>
+      </c>
+      <c r="L76" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M76" t="s">
+        <v>18</v>
+      </c>
+      <c r="O76" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P76" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q76" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R76" s="3">
+        <v>7</v>
+      </c>
+      <c r="S76" s="7">
+        <v>50</v>
+      </c>
+      <c r="T76" s="3">
+        <v>21</v>
+      </c>
+      <c r="U76" s="2">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="V76" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H77" s="3">
+        <v>100014</v>
+      </c>
+      <c r="I77" t="s">
+        <v>13</v>
+      </c>
+      <c r="J77" t="s">
+        <v>14</v>
+      </c>
+      <c r="K77" t="s">
+        <v>48</v>
+      </c>
+      <c r="L77" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="M77" t="s">
+        <v>18</v>
+      </c>
+      <c r="O77" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="P77" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q77" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R77" s="3">
+        <v>7</v>
+      </c>
+      <c r="S77" s="7">
+        <v>50</v>
+      </c>
+      <c r="T77" s="3">
+        <v>21</v>
+      </c>
+      <c r="U77" s="2">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="V77" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="I78" s="5"/>
+      <c r="O78"/>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="3"/>
+      <c r="T78" s="4"/>
+      <c r="U78" s="4"/>
+      <c r="V78" s="2"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="I79" s="5"/>
+      <c r="O79"/>
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="3"/>
+      <c r="T79" s="4"/>
+      <c r="U79" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="V79" s="2">
+        <f>AVERAGE(U50:U77)</f>
+        <v>1.9132142857142858</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B80" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="C80" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-      <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="4"/>
-      <c r="T52" s="4"/>
-    </row>
-    <row r="53" spans="1:20">
-      <c r="A53" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="4"/>
-    </row>
-    <row r="54" spans="1:20">
-      <c r="A54" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4"/>
-    </row>
-    <row r="55" spans="1:20">
-      <c r="A55" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="4"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-    </row>
-    <row r="56" spans="1:20">
-      <c r="A56" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-    </row>
-    <row r="57" spans="1:20">
-      <c r="A57" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-    </row>
-    <row r="58" spans="1:20">
-      <c r="A58" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="8"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-    </row>
-    <row r="59" spans="1:20">
-      <c r="D59" s="4"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="8"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-    </row>
-    <row r="60" spans="1:20">
-      <c r="A60" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="8"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-    </row>
-    <row r="61" spans="1:20">
-      <c r="A61" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="8"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-    </row>
-    <row r="62" spans="1:20">
-      <c r="A62" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-    </row>
-    <row r="63" spans="1:20">
-      <c r="A63" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-    </row>
-    <row r="64" spans="1:20">
-      <c r="A64" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="8"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-    </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="7"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3"/>
-      <c r="K66" s="3"/>
-      <c r="L66" s="7"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="8"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="3"/>
-    </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3"/>
-      <c r="K67" s="3"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="8"/>
-      <c r="O67" s="3"/>
-      <c r="P67" s="3"/>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="3"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="3"/>
-      <c r="P68" s="3"/>
-    </row>
-    <row r="69" spans="1:16">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="7"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="3"/>
-      <c r="P69" s="3"/>
-    </row>
-    <row r="70" spans="1:16">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="3"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="3"/>
-      <c r="P70" s="3"/>
-    </row>
-    <row r="71" spans="1:16">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="8"/>
-      <c r="O71" s="3"/>
-      <c r="P71" s="3"/>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3"/>
-      <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="3"/>
-      <c r="P72" s="3"/>
-    </row>
-    <row r="73" spans="1:16">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="3"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="3"/>
-      <c r="P73" s="3"/>
-    </row>
-    <row r="74" spans="1:16">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="7"/>
-      <c r="M74" s="3"/>
-      <c r="N74" s="8"/>
-      <c r="O74" s="3"/>
-      <c r="P74" s="3"/>
-    </row>
-    <row r="75" spans="1:16">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-      <c r="M75" s="3"/>
-      <c r="N75" s="8"/>
-      <c r="O75" s="3"/>
-      <c r="P75" s="3"/>
-    </row>
-    <row r="76" spans="1:16">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="8"/>
-      <c r="O76" s="3"/>
-      <c r="P76" s="3"/>
-    </row>
-    <row r="77" spans="1:16">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="7"/>
-      <c r="M77" s="3"/>
-      <c r="N77" s="8"/>
-      <c r="O77" s="3"/>
-      <c r="P77" s="3"/>
-    </row>
-    <row r="78" spans="1:16">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="8"/>
-      <c r="O78" s="3"/>
-      <c r="P78" s="3"/>
-    </row>
-    <row r="79" spans="1:16">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="8"/>
-      <c r="O79" s="3"/>
-      <c r="P79" s="3"/>
-    </row>
-    <row r="80" spans="1:16">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="7"/>
-      <c r="M80" s="3"/>
-      <c r="N80" s="8"/>
-      <c r="O80" s="3"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
       <c r="P80" s="3"/>
-    </row>
-    <row r="81" spans="1:16">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="3"/>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="3"/>
+      <c r="T80" s="4"/>
+      <c r="U80" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="V80" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="81" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B81" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E81" s="4"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="7"/>
+      <c r="L81" s="3"/>
       <c r="M81" s="3"/>
-      <c r="N81" s="8"/>
-      <c r="O81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="8"/>
       <c r="P81" s="3"/>
-    </row>
-    <row r="82" spans="1:16">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="3"/>
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="3"/>
+      <c r="T81" s="4"/>
+      <c r="U81" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="V81" s="2">
+        <f>V79/V80</f>
+        <v>6.8329081632653069E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B82" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
@@ -4423,52 +5994,68 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
       <c r="M82" s="3"/>
-      <c r="N82" s="8"/>
-      <c r="O82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="8"/>
       <c r="P82" s="3"/>
-    </row>
-    <row r="83" spans="1:16">
-      <c r="A83" s="4"/>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="4"/>
+      <c r="U82" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="V82" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="83" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B83" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="E83" s="4"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
-      <c r="L83" s="7"/>
+      <c r="L83" s="3"/>
       <c r="M83" s="3"/>
-      <c r="N83" s="8"/>
-      <c r="O83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="8"/>
       <c r="P83" s="3"/>
-    </row>
-    <row r="84" spans="1:16">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="3"/>
+      <c r="Q83" s="3"/>
+      <c r="S83" s="2"/>
+      <c r="V83" s="2"/>
+    </row>
+    <row r="84" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B84" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E84" s="4"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
-      <c r="L84" s="7"/>
+      <c r="L84" s="3"/>
       <c r="M84" s="3"/>
-      <c r="N84" s="8"/>
-      <c r="O84" s="3"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="8"/>
       <c r="P84" s="3"/>
-    </row>
-    <row r="85" spans="1:16">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="3"/>
+      <c r="Q84" s="3"/>
+      <c r="S84" s="2"/>
+      <c r="V84" s="2"/>
+    </row>
+    <row r="85" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="E85" s="4"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -4477,52 +6064,67 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
-      <c r="N85" s="8"/>
-      <c r="O85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="8"/>
       <c r="P85" s="3"/>
-    </row>
-    <row r="86" spans="1:16">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="3"/>
+      <c r="Q85" s="3"/>
+      <c r="S85" s="2"/>
+      <c r="V85" s="2"/>
+    </row>
+    <row r="86" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B86" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E86" s="4"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
-      <c r="L86" s="7"/>
+      <c r="L86" s="3"/>
       <c r="M86" s="3"/>
-      <c r="N86" s="8"/>
-      <c r="O86" s="3"/>
+      <c r="N86" s="3"/>
+      <c r="O86" s="8"/>
       <c r="P86" s="3"/>
-    </row>
-    <row r="87" spans="1:16">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="S86" s="2"/>
+      <c r="V86" s="2"/>
+    </row>
+    <row r="87" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B87" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
-      <c r="L87" s="7"/>
+      <c r="L87" s="3"/>
       <c r="M87" s="3"/>
-      <c r="N87" s="8"/>
-      <c r="O87" s="3"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="8"/>
       <c r="P87" s="3"/>
-    </row>
-    <row r="88" spans="1:16">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="S87" s="2"/>
+      <c r="V87" s="2"/>
+    </row>
+    <row r="88" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B88" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="E88" s="4"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -4531,261 +6133,182 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
       <c r="M88" s="3"/>
-      <c r="N88" s="8"/>
-      <c r="O88" s="3"/>
+      <c r="N88" s="3"/>
+      <c r="O88" s="8"/>
       <c r="P88" s="3"/>
-    </row>
-    <row r="89" spans="1:16">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-      <c r="L89" s="7"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="8"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
-    </row>
-    <row r="90" spans="1:16">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
-      <c r="M90" s="3"/>
-      <c r="N90" s="8"/>
-      <c r="O90" s="3"/>
-      <c r="P90" s="3"/>
-    </row>
-    <row r="91" spans="1:16">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
+      <c r="Q88" s="3"/>
+      <c r="S88" s="2"/>
+      <c r="V88" s="2"/>
+    </row>
+    <row r="91" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B91" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
-      <c r="M91" s="3"/>
-      <c r="N91" s="8"/>
-      <c r="O91" s="3"/>
-      <c r="P91" s="3"/>
-    </row>
-    <row r="92" spans="1:16">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="3"/>
+    </row>
+    <row r="92" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B92" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
-      <c r="N92" s="8"/>
-      <c r="O92" s="3"/>
-      <c r="P92" s="3"/>
-    </row>
-    <row r="93" spans="1:16">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="4"/>
-      <c r="E93" s="3"/>
+    </row>
+    <row r="93" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B93" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E93" s="4"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
-      <c r="M93" s="3"/>
-      <c r="N93" s="8"/>
-      <c r="O93" s="3"/>
-      <c r="P93" s="3"/>
-    </row>
-    <row r="94" spans="1:16">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="4"/>
-      <c r="E94" s="3"/>
+    </row>
+    <row r="94" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B94" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="E94" s="4"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="7"/>
-      <c r="M94" s="3"/>
-      <c r="N94" s="8"/>
-      <c r="O94" s="3"/>
-      <c r="P94" s="3"/>
-    </row>
-    <row r="95" spans="1:16">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="3"/>
+    </row>
+    <row r="95" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B95" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" s="4"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="8"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-    </row>
-    <row r="96" spans="1:16">
-      <c r="A96" s="4"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="4"/>
-      <c r="E96" s="3"/>
+    </row>
+    <row r="96" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B96" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E96" s="4"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="8"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-    </row>
-    <row r="97" spans="1:16">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="3"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B97" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="8"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-    </row>
-    <row r="98" spans="1:16">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="4"/>
-      <c r="E98" s="3"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E98" s="4"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="8"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-    </row>
-    <row r="99" spans="1:16">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="3"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B99" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E99" s="4"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="8"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-    </row>
-    <row r="100" spans="1:16">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
-      <c r="E100" s="3"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B100" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="4"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="8"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-    </row>
-    <row r="101" spans="1:16">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
-      <c r="E101" s="3"/>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B101" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E101" s="4"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="8"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-    </row>
-    <row r="102" spans="1:16">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B102" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E102" s="4"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="I102" s="4"/>
-      <c r="J102" s="4"/>
-      <c r="K102" s="4"/>
-      <c r="L102" s="4"/>
-      <c r="M102" s="4"/>
-      <c r="N102" s="4"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B103" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="E103" s="4"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B104" s="4"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B105" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="4"/>
+      <c r="E105" s="4"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>